<commit_message>
Final Frame work ready commit
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F5733A58-7C3E-4942-9A11-39916541650A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{12B1FA1D-83A5-4F06-9901-A678A4B74E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -414,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -564,7 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>